<commit_message>
Fixed bug in price discount
</commit_message>
<xml_diff>
--- a/Proyecto_Integrador_-_Jugueteria_Cosmica_-_Etapa_2_-_Consignas_cumplidas.xlsx
+++ b/Proyecto_Integrador_-_Jugueteria_Cosmica_-_Etapa_2_-_Consignas_cumplidas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="116">
   <si>
     <t xml:space="preserve">Consigna</t>
   </si>
@@ -37,7 +37,6 @@
         <color rgb="FF491347"/>
         <rFont val="Century Gothic"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Proyecto Integrador: </t>
     </r>
@@ -48,7 +47,6 @@
         <color rgb="FF491347"/>
         <rFont val="Century Gothic"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Juguetería Cósmica</t>
     </r>
@@ -76,17 +74,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Fecha máxima para presentar el proyecto: martes 02/08/2022 en cualquier horario.</t>
     </r>
@@ -111,17 +107,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Pueden utilizar Google Fonts, Font Awesome o similares.</t>
     </r>
@@ -143,17 +137,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Pueden incorporar otros elementos como imágenes, videos, archivos de tipografías, etc.</t>
     </r>
@@ -175,17 +167,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Todos los archivos deben pasar las validaciones de la W3C.</t>
     </r>
@@ -207,17 +197,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">No se permite el uso de Bootstrap ni de jQuery.</t>
     </r>
@@ -239,17 +227,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Pueden utilizar cualquier tipo de técnica, lo hayamos visto o no en clase.</t>
     </r>
@@ -271,17 +257,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Es requerido utilizar un diseño responsive en todas las páginas del proyecto. Se tendrán que tener en cuenta no solo las resoluciones chicas y medianas, sino también las extra grandes, manteniendo el orden, estructura y estética del sitio en todo tipo de resolución. Cuidar especialmente las proporciones de cada elemento en cada resolución y en relación al resto de los componentes de la página.</t>
     </r>
@@ -303,17 +287,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Deberán asegurarse de que el proyecto funcione con o sin Live Server.</t>
     </r>
@@ -335,17 +317,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Deberá utilizarse SASS y el patrón 7-1, con nomenclatura BEM y nombres de clases en inglés. Se requiere utilizar, como mínimo, los archivos de SASS ya definidos, si bien se podrán adicionar otros. Todos los estilos utilizados deberán ser escritos en archivos SCSS. El proyecto se deberá entregar con el archivo "main.css" ya compilado, pero el mismo se podrá borrar una vez recibido el proyecto y verificar que el archivo "main.scss", al compilarse, vuelva a generar el archivo CSS mencionado.</t>
     </r>
@@ -367,17 +347,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Deberán utilizar JavaScript Vanilla (es decir, sin el uso de librerías externas).</t>
     </r>
@@ -399,17 +377,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Se sugiere utilizar Git para el desarrollo, si bien no es un requisito para esta primera etapa.</t>
     </r>
@@ -434,17 +410,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Cumpliendo con las especificaciones planteadas a lo largo de este documento, la elección de estilos de CSS de todas las páginas queda a elección de cada alumno.</t>
     </r>
@@ -565,17 +539,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Fecha máxima para presentar el proyecto: jueves 22/09/2022 en cualquier horario.</t>
     </r>
@@ -597,17 +569,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Todo el contenido desarrollado para esta segunda etapa deberá ser compatible con lo solicitado para la primera. Siguiendo con esa línea, podrán continuar haciendo todos los cambios que crean pertinentes o que no hayan llegado a hacer para la primera etapa. Esto incluye modificaciones en los estilos, agregado de elementos en las distintas vistas o incluso un rediseño completo, siempre y cuando se cumplan con todos los requisitos detallados para ambas etapas.</t>
     </r>
@@ -629,17 +599,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">No se requiere utilizar Node.js en esta entrega. Sin embargo, se admite su uso. En caso de utilizarlo, Los archivos entregados no deberán incluir el directorio con los node modules, pero sí el package.json correspondiente.</t>
     </r>
@@ -664,17 +632,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Deberá elaborarse una SPA que permita acceder a cada una de las vistas, recargando solo el contenido del elemento &lt;main&gt;, manteniendo en todo momento los elementos &lt;header&gt; y &lt;footer&gt; (hijos de &lt;body&gt;) en el DOM, es decir, sin recargarlos.</t>
     </r>
@@ -696,17 +662,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">La comunicación con el servidor puede intercambiar datos de cualquier tipo, ya sea texto o HTML crudo, JSON, archivos binarios, etc, en cualquier vista. Podrán obtenerse datos del servidor, de forma asincrónica, no solo para las vistas principales, sino en cualquier momento en donde se requiera.</t>
     </r>
@@ -728,17 +692,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Se podrá utilizará Live Server o Node.js + Express como servidor web (solo uno de ellos), a elección del alumno.</t>
     </r>
@@ -760,17 +722,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Deberá utilizarse fetch() con async/await para las conexiones asincrónicas con el servidor.</t>
     </r>
@@ -792,17 +752,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Al navegar por el sitio la URL debe ir cambiando. Todas las URL visibles por el usuario deben ser amigables y al acceder directamente a una deberá mostrarse el contenido correspondiente. Idealmente destacar de alguna manera el vínculo correspondiente a la vista activa.</t>
     </r>
@@ -824,22 +782,122 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Todas las acciones que vaya realizando el usuario deben brindar algún tipo de feedback. Ej: los vínculos y botones deben reaccionar ante hover, focus y active, etc.</t>
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Debe tenerse en cuenta que no todas las personas razonan igual, por lo que no siempre van a entender lo mismo ante los mismos elementos, por lo que es buena idea agregar ayudas contextuales, como atributos title, mensajes emergentes, u otro tipo de indicadores que marquen qué sucede al presionar tal botón o luego de realizar ciertas acciones, etc.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Todas las acciones se deben poder realizar en cualquier resolución de pantalla y tipo de dispositivo. No olvidar los distintos tipos de interacción que existen en cada tipo de dispositivo (ej: pocos dispositivos táctiles reaccionan ante el hover). Recordar acomodar los elementos apropiadamente no solo en resoluciones chicas y medias, sino también en resoluciones muy grandes.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Elementos comunes a todo el sitio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Botón de carrito</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ubicado físicamente dentro del elemento &lt;header&gt; del &lt;body&gt;, podrá mostrarse arriba o en cualquier lugar de la página, gracias a los distintos mecanismos que CSS provee para tal fin. El botón deberá mostrar y ocultar, de manera alternada, un contenedor del tipo </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">modal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> en el que se verá el listado de productos que se hayan agregado al carrito.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Carrito modal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se mostrará cuando el botón del carrito del header sea presionado.</t>
+  </si>
+  <si>
     <t xml:space="preserve">No</t>
   </si>
   <si>
@@ -847,81 +905,10 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t xml:space="preserve">·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Debe tenerse en cuenta que no todas las personas razonan igual, por lo que no siempre van a entender lo mismo ante los mismos elementos, por lo que es buena idea agregar ayudas contextuales, como atributos title, mensajes emergentes, u otro tipo de indicadores que marquen qué sucede al presionar tal botón o luego de realizar ciertas acciones, etc.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t xml:space="preserve">·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Todas las acciones se deben poder realizar en cualquier resolución de pantalla y tipo de dispositivo. No olvidar los distintos tipos de interacción que existen en cada tipo de dispositivo (ej: pocos dispositivos táctiles reaccionan ante el hover). Recordar acomodar los elementos apropiadamente no solo en resoluciones chicas y medias, sino también en resoluciones muy grandes.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Elementos comunes a todo el sitio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Botón de carrito</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Ubicado físicamente dentro del elemento &lt;header&gt; del &lt;body&gt;, podrá mostrarse arriba o en cualquier lugar de la página, gracias a los distintos mecanismos que CSS provee para tal fin. El botón deberá mostrar y ocultar, de manera alternada, un contenedor del tipo </t>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">El diseño y tamaño del modal es libre, pudiendo incorporarse de manera centrada, en un lateral, etc. En todos los casos deberá funcionar como </t>
     </r>
     <r>
       <rPr>
@@ -930,7 +917,6 @@
         <color rgb="FF000000"/>
         <rFont val="Century Gothic"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">modal</t>
     </r>
@@ -940,46 +926,6 @@
         <color rgb="FF000000"/>
         <rFont val="Century Gothic"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> en el que se verá el listado de productos que se hayan agregado al carrito.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Carrito modal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se mostrará cuando el botón del carrito del header sea presionado.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">El diseño y tamaño del modal es libre, pudiendo incorporarse de manera centrada, en un lateral, etc. En todos los casos deberá funcionar como </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">modal</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, por encima de los demás elementos de la página, de manera flotante.</t>
     </r>
@@ -1004,17 +950,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Presionando nuevamente en el botón del carrito</t>
     </r>
@@ -1036,17 +980,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Presionando en una x de cierre incorporada dentro del modal</t>
     </r>
@@ -1068,17 +1010,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Presionando la tecla ESC del teclado</t>
     </r>
@@ -1100,17 +1040,15 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Haciendo click en cualquier zona fuera del modal.</t>
     </r>
@@ -1246,7 +1184,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1268,21 +1205,18 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="18"/>
       <color rgb="FF491347"/>
       <name val="Century Gothic"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -1290,14 +1224,12 @@
       <color rgb="FF491347"/>
       <name val="Century Gothic"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="16"/>
       <color rgb="FF6D1D6A"/>
       <name val="Century Gothic"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1311,35 +1243,30 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Century Gothic"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF6D1D6A"/>
       <name val="Century Gothic"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF6D1D6A"/>
       <name val="Century Gothic"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF6D1D6A"/>
       <name val="Century Gothic"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -1347,7 +1274,6 @@
       <color rgb="FF000000"/>
       <name val="Century Gothic"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1474,7 +1400,10 @@
   <dxfs count="3">
     <dxf>
       <font>
+        <name val="Calibri"/>
+        <family val="2"/>
         <color rgb="FFC00000"/>
+        <sz val="11"/>
       </font>
       <fill>
         <patternFill>
@@ -1484,7 +1413,10 @@
     </dxf>
     <dxf>
       <font>
+        <name val="Calibri"/>
+        <family val="2"/>
         <color rgb="FF006100"/>
+        <sz val="11"/>
       </font>
       <fill>
         <patternFill>
@@ -1493,6 +1425,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFE7E6E6"/>
@@ -1571,19 +1509,19 @@
   <dimension ref="A1:C116"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="112"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="94.29"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1594,13 +1532,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -1612,7 +1550,7 @@
       </c>
       <c r="B4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
@@ -1620,7 +1558,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
@@ -1628,7 +1566,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1636,7 +1574,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
         <v>10</v>
       </c>
@@ -1644,7 +1582,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
         <v>11</v>
       </c>
@@ -1652,7 +1590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
@@ -1660,7 +1598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="66" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
@@ -1668,7 +1606,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
@@ -1676,7 +1614,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
@@ -1684,7 +1622,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
@@ -1703,7 +1641,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
         <v>19</v>
       </c>
@@ -1717,7 +1655,7 @@
       </c>
       <c r="B17" s="5"/>
     </row>
-    <row r="18" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
         <v>21</v>
       </c>
@@ -1725,13 +1663,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="5"/>
     </row>
-    <row r="20" customFormat="false" ht="49.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
         <v>23</v>
       </c>
@@ -1739,7 +1677,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
         <v>24</v>
       </c>
@@ -1747,7 +1685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
         <v>25</v>
       </c>
@@ -1755,13 +1693,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="5"/>
     </row>
-    <row r="24" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
         <v>27</v>
       </c>
@@ -1769,7 +1707,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
         <v>28</v>
       </c>
@@ -1777,7 +1715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
         <v>29</v>
       </c>
@@ -1785,7 +1723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
         <v>30</v>
       </c>
@@ -1793,7 +1731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
         <v>31</v>
       </c>
@@ -1801,13 +1739,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B29" s="5"/>
     </row>
-    <row r="30" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
         <v>33</v>
       </c>
@@ -1815,13 +1753,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="5"/>
     </row>
-    <row r="32" customFormat="false" ht="49.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
         <v>35</v>
       </c>
@@ -1829,13 +1767,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B33" s="5"/>
     </row>
-    <row r="34" customFormat="false" ht="66" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
         <v>37</v>
       </c>
@@ -1843,13 +1781,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B35" s="5"/>
     </row>
-    <row r="36" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
         <v>39</v>
       </c>
@@ -1857,7 +1795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
         <v>40</v>
       </c>
@@ -1865,19 +1803,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="5"/>
-    </row>
-    <row r="39" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B39" s="5"/>
     </row>
-    <row r="40" customFormat="false" ht="49.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
         <v>43</v>
       </c>
@@ -1885,13 +1825,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B41" s="5"/>
     </row>
-    <row r="42" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
         <v>45</v>
       </c>
@@ -1899,13 +1839,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="11" t="s">
         <v>46</v>
       </c>
       <c r="B43" s="5"/>
     </row>
-    <row r="44" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
         <v>47</v>
       </c>
@@ -1913,13 +1853,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="66" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B45" s="5"/>
     </row>
-    <row r="46" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
         <v>49</v>
       </c>
@@ -1927,13 +1867,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="s">
         <v>50</v>
       </c>
       <c r="B47" s="5"/>
     </row>
-    <row r="48" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
         <v>51</v>
       </c>
@@ -1941,7 +1881,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
         <v>52</v>
       </c>
@@ -1953,13 +1893,13 @@
       </c>
       <c r="B50" s="5"/>
     </row>
-    <row r="51" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B51" s="5"/>
     </row>
-    <row r="52" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="8" t="s">
         <v>54</v>
       </c>
@@ -1967,7 +1907,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="49.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="8" t="s">
         <v>55</v>
       </c>
@@ -1981,7 +1921,7 @@
       </c>
       <c r="B54" s="5"/>
     </row>
-    <row r="55" customFormat="false" ht="49.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="8" t="s">
         <v>57</v>
       </c>
@@ -1997,7 +1937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="8" t="s">
         <v>59</v>
       </c>
@@ -2005,7 +1945,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="8" t="s">
         <v>60</v>
       </c>
@@ -2013,7 +1953,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="49.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="8" t="s">
         <v>61</v>
       </c>
@@ -2026,18 +1966,18 @@
         <v>62</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="5"/>
+    </row>
+    <row r="62" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="B61" s="5"/>
-    </row>
-    <row r="62" customFormat="false" ht="66" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>7</v>
@@ -2045,39 +1985,39 @@
     </row>
     <row r="63" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63" s="5"/>
+    </row>
+    <row r="64" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="B63" s="5"/>
-    </row>
-    <row r="64" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="B64" s="5"/>
     </row>
     <row r="65" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B65" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="10" t="s">
+      <c r="B66" s="5"/>
+    </row>
+    <row r="67" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B66" s="5"/>
-    </row>
-    <row r="67" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="9" t="s">
+      <c r="B67" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B67" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="49.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="68" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="9" t="s">
         <v>71</v>
       </c>
@@ -2085,21 +2025,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="9" t="s">
         <v>72</v>
       </c>
       <c r="B69" s="5"/>
     </row>
-    <row r="70" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="8" t="s">
         <v>73</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="8" t="s">
         <v>74</v>
       </c>
@@ -2107,7 +2047,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="8" t="s">
         <v>75</v>
       </c>
@@ -2115,7 +2055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="8" t="s">
         <v>76</v>
       </c>
@@ -2123,15 +2063,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="66" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="9" t="s">
         <v>77</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="99" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="9" t="s">
         <v>78</v>
       </c>
@@ -2145,7 +2085,7 @@
       </c>
       <c r="B76" s="5"/>
     </row>
-    <row r="77" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="9" t="s">
         <v>80</v>
       </c>
@@ -2153,13 +2093,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="10" t="s">
         <v>81</v>
       </c>
       <c r="B78" s="5"/>
     </row>
-    <row r="79" customFormat="false" ht="132" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="9" t="s">
         <v>82</v>
       </c>
@@ -2167,7 +2107,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="66" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="9" t="s">
         <v>83</v>
       </c>
@@ -2175,7 +2115,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="66" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="9" t="s">
         <v>84</v>
       </c>
@@ -2183,27 +2123,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="10" t="s">
         <v>85</v>
       </c>
       <c r="B82" s="5"/>
     </row>
-    <row r="83" customFormat="false" ht="132" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="9" t="s">
         <v>86</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="11" t="s">
         <v>87</v>
       </c>
       <c r="B84" s="5"/>
     </row>
-    <row r="85" customFormat="false" ht="49.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="9" t="s">
         <v>88</v>
       </c>
@@ -2211,13 +2151,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="11" t="s">
         <v>89</v>
       </c>
       <c r="B86" s="5"/>
     </row>
-    <row r="87" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="9" t="s">
         <v>90</v>
       </c>
@@ -2225,13 +2165,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="11" t="s">
         <v>91</v>
       </c>
       <c r="B88" s="5"/>
     </row>
-    <row r="89" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="9" t="s">
         <v>92</v>
       </c>
@@ -2239,13 +2179,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="11" t="s">
         <v>93</v>
       </c>
       <c r="B90" s="5"/>
     </row>
-    <row r="91" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="9" t="s">
         <v>94</v>
       </c>
@@ -2253,13 +2193,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="11" t="s">
         <v>95</v>
       </c>
       <c r="B92" s="5"/>
     </row>
-    <row r="93" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="9" t="s">
         <v>96</v>
       </c>
@@ -2267,13 +2207,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="11" t="s">
         <v>97</v>
       </c>
       <c r="B94" s="5"/>
     </row>
-    <row r="95" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="9" t="s">
         <v>98</v>
       </c>
@@ -2281,13 +2221,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="11" t="s">
         <v>99</v>
       </c>
       <c r="B96" s="5"/>
     </row>
-    <row r="97" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="9" t="s">
         <v>100</v>
       </c>
@@ -2295,13 +2235,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="11" t="s">
         <v>101</v>
       </c>
       <c r="B98" s="5"/>
     </row>
-    <row r="99" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="9" t="s">
         <v>102</v>
       </c>
@@ -2309,7 +2249,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="9" t="s">
         <v>103</v>
       </c>
@@ -2323,7 +2263,7 @@
       </c>
       <c r="B101" s="5"/>
     </row>
-    <row r="102" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="9" t="s">
         <v>105</v>
       </c>
@@ -2337,7 +2277,7 @@
       </c>
       <c r="B103" s="5"/>
     </row>
-    <row r="104" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="9" t="s">
         <v>105</v>
       </c>
@@ -2345,19 +2285,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="9" t="s">
         <v>107</v>
       </c>
       <c r="B105" s="5"/>
     </row>
-    <row r="106" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="11" t="s">
         <v>108</v>
       </c>
       <c r="B106" s="5"/>
     </row>
-    <row r="107" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="9" t="s">
         <v>109</v>
       </c>
@@ -2365,13 +2305,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="10" t="s">
         <v>110</v>
       </c>
       <c r="B108" s="5"/>
     </row>
-    <row r="109" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="9" t="s">
         <v>111</v>
       </c>
@@ -2379,19 +2319,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="9" t="s">
         <v>112</v>
       </c>
       <c r="B110" s="5"/>
     </row>
-    <row r="111" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="11" t="s">
         <v>87</v>
       </c>
       <c r="B111" s="5"/>
     </row>
-    <row r="112" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="9" t="s">
         <v>113</v>
       </c>
@@ -2399,13 +2339,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="11" t="s">
         <v>114</v>
       </c>
       <c r="B113" s="5"/>
     </row>
-    <row r="114" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="9" t="s">
         <v>113</v>
       </c>
@@ -2413,13 +2353,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="11" t="s">
         <v>115</v>
       </c>
       <c r="B115" s="5"/>
     </row>
-    <row r="116" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="9" t="s">
         <v>113</v>
       </c>
@@ -2442,12 +2382,12 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" error="Se debe ingresar exactamente &quot;Sí&quot; o &quot;No&quot;" errorStyle="stop" errorTitle="Solo &quot;Sí&quot; o &quot;No&quot;" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2:B1116" type="list">
-      <formula1>"Sí,No"</formula1>
+    <dataValidation allowBlank="true" error="Se debe ingresar exactamente &quot;Sí&quot; o &quot;No&quot;" errorStyle="stop" errorTitle="Solo &quot;Sí&quot; o &quot;No&quot;" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1" type="none">
+      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Se debe ingresar exactamente &quot;Sí&quot; o &quot;No&quot;" errorStyle="stop" errorTitle="Solo &quot;Sí&quot; o &quot;No&quot;" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1" type="none">
-      <formula1>0</formula1>
+    <dataValidation allowBlank="true" error="Se debe ingresar exactamente &quot;Sí&quot; o &quot;No&quot;" errorStyle="stop" errorTitle="Solo &quot;Sí&quot; o &quot;No&quot;" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2:B1116" type="list">
+      <formula1>"Sí,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>